<commit_message>
feat: Implement unique identifier in sample data and mapping JSON config files, and update code to handle it
</commit_message>
<xml_diff>
--- a/dist/data/input/sample.xlsx
+++ b/dist/data/input/sample.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+  <si>
+    <t>ExcelId</t>
+  </si>
   <si>
     <t>ExcelProductName</t>
   </si>
@@ -31,7 +34,10 @@
     <t>ExcelDiscount</t>
   </si>
   <si>
-    <t>Widget Excel A</t>
+    <t>d0a8bec1-2690-437c-b857-3a399df25b83</t>
+  </si>
+  <si>
+    <t>Widget Excel A update</t>
   </si>
   <si>
     <t>19.99</t>
@@ -44,6 +50,9 @@
   </si>
   <si>
     <t>5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Widget Excel B</t>
@@ -417,7 +426,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -428,6 +437,7 @@
     <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -446,56 +456,66 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>